<commit_message>
Módulo 11 - Fórmulas avançadas (SOMARPRODUTOS)
</commit_message>
<xml_diff>
--- a/Módulo 11 - Formulas avançadas/aula-desloc-corresp.xlsx
+++ b/Módulo 11 - Formulas avançadas/aula-desloc-corresp.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="8670" windowHeight="6780" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Estados" sheetId="1" r:id="rId1"/>
@@ -16,6 +16,9 @@
     <externalReference r:id="rId5"/>
   </externalReferences>
   <definedNames>
+    <definedName name="Cidades">TbCidades[Cidade]</definedName>
+    <definedName name="Estado">TbCidades[Estado]</definedName>
+    <definedName name="Estados">TbEstados[Estado]</definedName>
     <definedName name="TbCidades_Cidade">[1]!TbCidades[Cidade]</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
@@ -23,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="42">
   <si>
     <t>Estado</t>
   </si>
@@ -91,9 +94,6 @@
     <t>Classificação</t>
   </si>
   <si>
-    <t>Secundárias</t>
-  </si>
-  <si>
     <t>DESLOC</t>
   </si>
   <si>
@@ -125,6 +125,33 @@
   </si>
   <si>
     <t>Valor</t>
+  </si>
+  <si>
+    <t>Corresp : retorna a posição da primeira ocorrência do valor procurado</t>
+  </si>
+  <si>
+    <t>=DESLOC(Cidades;D6-1;0;D9)</t>
+  </si>
+  <si>
+    <t>O 0 representa que ele não irá permanecer na da coluna, o último atributo revela a quantidade</t>
+  </si>
+  <si>
+    <t>de linhas que aparecerá na lista</t>
+  </si>
+  <si>
+    <t>=CORRESP(D3;Estado;0)</t>
+  </si>
+  <si>
+    <t>D3 é o valor procurado, estado é o intervalo onde o valor será procurado, e 0 significa que o valor deve ser idêntico e não aproximado</t>
+  </si>
+  <si>
+    <t>O D6 pega a formula que encontra a quantidade de ocorrências do valor passado na célula acima(numero de linhas que será percorrido)</t>
+  </si>
+  <si>
+    <t>=DESLOC(ref;linhas;colunas)</t>
+  </si>
+  <si>
+    <t>A fórmula afirma que haverá um deslocamento na coluna de Cidades ( intervalo) onde os dados seram procurados. O cidades é o ponto de referencia onde irá iniciar o processo de deslocamento</t>
   </si>
 </sst>
 </file>
@@ -132,7 +159,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;* #,##0.00_-;\-&quot;R$&quot;* #,##0.00_-;_-&quot;R$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-&quot;R$&quot;* #,##0.00_-;\-&quot;R$&quot;* #,##0.00_-;_-&quot;R$&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -217,9 +244,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -247,13 +274,18 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
-      <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;* #,##0.00_-;\-&quot;R$&quot;* #,##0.00_-;_-&quot;R$&quot;* &quot;-&quot;??_-;_-@_-"/>
+      <numFmt numFmtId="164" formatCode="_-&quot;R$&quot;* #,##0.00_-;\-&quot;R$&quot;* #,##0.00_-;_-&quot;R$&quot;* &quot;-&quot;??_-;_-@_-"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -311,8 +343,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="TbRepasses" displayName="TbRepasses" ref="A1:C4" totalsRowShown="0">
-  <autoFilter ref="A1:C4"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="TbRepasses" displayName="TbRepasses" ref="A1:C6" totalsRowShown="0">
+  <autoFilter ref="A1:C6"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Estado"/>
     <tableColumn id="2" name="Cidade"/>
@@ -611,7 +643,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A6"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -658,16 +692,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
+    <sheetView topLeftCell="A2" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
     <col min="2" max="2" width="26" customWidth="1"/>
     <col min="4" max="4" width="19.42578125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="18" customWidth="1"/>
+    <col min="6" max="6" width="23.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -686,9 +722,11 @@
         <v>7</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F2" s="5"/>
+        <v>24</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -708,7 +746,9 @@
       <c r="B4" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="5"/>
+      <c r="F4" s="5" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -718,7 +758,7 @@
         <v>10</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -728,8 +768,13 @@
       <c r="B6" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="3"/>
-      <c r="F6" s="5"/>
+      <c r="D6" s="3">
+        <f>MATCH(D3,Estado,0)</f>
+        <v>3</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -747,7 +792,7 @@
         <v>13</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -757,7 +802,10 @@
       <c r="B9" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="3"/>
+      <c r="D9" s="3">
+        <f>COUNTIF(Estado,D3)</f>
+        <v>4</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -815,7 +863,63 @@
         <v>5</v>
       </c>
     </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G18" s="14" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B19" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="G19" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20" s="15"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="15"/>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B24" s="14" t="s">
+        <v>40</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B20:F20"/>
+  </mergeCells>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2">
+      <formula1>OFFSET(Cidades,4,0,3)</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4">
+      <formula1>OFFSET(Cidades,D6-1,0,3)</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F6">
+      <formula1>OFFSET(Cidades,D6-1,0,D9)</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -825,9 +929,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -852,7 +958,7 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="C2" s="1">
         <v>80000</v>
@@ -874,13 +980,43 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="C4" s="1">
         <v>40000</v>
       </c>
     </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="1">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="1">
+        <v>23567</v>
+      </c>
+    </row>
   </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A6">
+      <formula1>Estados</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B6">
+      <formula1>OFFSET(Cidades, MATCH(A2,Estado, 0)-1, 0, COUNTIF(Estado,A2))</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -890,10 +1026,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -902,117 +1038,141 @@
     <col min="2" max="2" width="11.7109375" style="10" customWidth="1"/>
     <col min="4" max="4" width="20.28515625" customWidth="1"/>
     <col min="6" max="6" width="23.42578125" customWidth="1"/>
+    <col min="10" max="10" width="4.7109375" customWidth="1"/>
+    <col min="11" max="11" width="4.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>21</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" t="s">
         <v>23</v>
       </c>
-      <c r="F1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B2" s="8">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B3" s="8">
         <v>2</v>
       </c>
       <c r="D3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" t="s">
         <v>28</v>
       </c>
-      <c r="F3" t="s">
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="12" t="s">
         <v>29</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
-        <v>30</v>
       </c>
       <c r="B4" s="8">
         <v>3</v>
       </c>
-      <c r="D4" s="5"/>
+      <c r="D4" s="5">
+        <f ca="1">OFFSET(A5,3,1)</f>
+        <v>7</v>
+      </c>
       <c r="F4" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B5" s="8">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D5">
+        <f ca="1">SUM(OFFSET(A5,3,1,3))</f>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B6" s="8">
         <v>5</v>
       </c>
       <c r="F6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B7" s="8">
         <v>6</v>
       </c>
-      <c r="F7" s="6"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F7" s="6">
+        <f>MATCH(F4,A2:A11,0)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B8" s="8">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B9" s="8">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B10" s="8">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F10" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="13"/>
+      <c r="K10" s="13"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B11" s="9">
         <v>10</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="F10:K10"/>
+  </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>